<commit_message>
updated LoginPage_Test.java file with some changes in other files.
</commit_message>
<xml_diff>
--- a/testdata/Login.xlsx
+++ b/testdata/Login.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sameer\Title21Automation\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView windowHeight="5970" windowWidth="15540" xWindow="0" yWindow="0"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L17"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,13 +32,13 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>Invalid password</t>
-  </si>
-  <si>
     <t>administrator</t>
   </si>
   <si>
-    <t xml:space="preserve">Valid </t>
+    <t>Test Invalid password</t>
+  </si>
+  <si>
+    <t>Test valid password</t>
   </si>
 </sst>
 </file>
@@ -372,17 +376,25 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="17.0" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -390,31 +402,31 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
finalized Login and Logout functionality.
</commit_message>
<xml_diff>
--- a/testdata/Login.xlsx
+++ b/testdata/Login.xlsx
@@ -385,13 +385,13 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="17.0" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated files and excel
</commit_message>
<xml_diff>
--- a/testdata/Login.xlsx
+++ b/testdata/Login.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sameer\Title21Automation\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neosoft\git\Title21Automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="5970" windowWidth="15540" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" windowHeight="5835" windowWidth="6285" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
+    <sheet name="GroupDetails" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>sysadmin</t>
   </si>
@@ -39,6 +40,18 @@
   </si>
   <si>
     <t>Test valid password</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Test123</t>
   </si>
 </sst>
 </file>
@@ -375,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,4 +447,35 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>